<commit_message>
template updated, added Irrelevant filter
</commit_message>
<xml_diff>
--- a/Projects/DIAGEOGTR/Data/set_up.xlsx
+++ b/Projects/DIAGEOGTR/Data/set_up.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Functional KPIs" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Functional KPIs'!$A$1:$G$2</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Functional KPIs'!$A$1:$G$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Functional KPIs'!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Functional KPIs'!$A$1:$F$2</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t xml:space="preserve">KPI Type</t>
   </si>
   <si>
-    <t xml:space="preserve">Channel</t>
-  </si>
-  <si>
     <t xml:space="preserve">Scene type / Tasks</t>
   </si>
   <si>
@@ -44,19 +41,13 @@
     <t xml:space="preserve">Include Empty</t>
   </si>
   <si>
-    <t xml:space="preserve">Exclude SKUs</t>
+    <t xml:space="preserve">Include Irrelevant</t>
   </si>
   <si>
     <t xml:space="preserve">GTR_SKU_FACINGS_BY_SCENE</t>
   </si>
   <si>
-    <t xml:space="preserve">01_Primary Shelf (Bi-Weekly), 01_Primary Shelf (Bi-Weekly)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Include </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exclude</t>
   </si>
 </sst>
 </file>
@@ -66,7 +57,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -96,6 +87,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="14"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -184,16 +182,16 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -282,30 +280,29 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="29.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="51.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="16.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1009" min="8" style="1" width="8.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1019" min="1010" style="0" width="8.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1020" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="51.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1008" min="7" style="1" width="8.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1018" min="1009" style="0" width="8.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1019" style="0" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="45.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" s="5" customFormat="true" ht="45.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -314,37 +311,35 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="AME1" s="0"/>
       <c r="AMF1" s="0"/>
       <c r="AMG1" s="0"/>
       <c r="AMH1" s="0"/>
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
-    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G2"/>
+  <autoFilter ref="A1:F1"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Template updated with scene-types
</commit_message>
<xml_diff>
--- a/Projects/DIAGEOGTR/Data/set_up.xlsx
+++ b/Projects/DIAGEOGTR/Data/set_up.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Functional KPIs" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Functional KPIs'!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Functional KPIs'!$A$1:$F$2</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Functional KPIs'!$A$1:$F$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Functional KPIs'!$A$1:$F$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t xml:space="preserve">KPI Type</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t xml:space="preserve">GTR_SKU_FACINGS_BY_SCENE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirits Permanent Gondola- Inactive, Spirits Other Permanent placements-Inactive, Spirits Permanent Cashier/POS - Inactive, Spirits promotional space in store- Inactive, Spirits promotional space concourse- Inactive, Spirits Shop In Shop- Inactive, Spirits Stand Alone Store- Inactive, Spirits Permanent – Wall bay APAC, Spirits Permanent – Wall bay Americas, Spirits Permanent – Wall bay Europe, Spirits Permanent – Wall bay MENA, Spirits Other Permanent placements APAC, Spirits Other Permanent placements Americas, Spirits Other Permanent placements Europe, Spirits Other Permanent placements MENA, Spirits Permanent Cashier/POS APAC, Spirits Permanent Cashier/POS Americas, Spirits Permanent Cashier/POS Europe, Spirits Permanent Cashier/POS MENA, Spirits Permanent Gondola APAC, Spirits Permanent Gondola Americas, Spirits Permanent Gondola Europe, Spirits Permanent Gondola MENA, Spirits promotional space concourse APAC, Spirits promotional space concourse Americas, Spirits promotional space concourse Europe, Spirits promotional space concourse MENA, Spirits promotional space in store APAC, Spirits promotional space in store Americas, Spirits promotional space in store Europe, Spirits promotional space in store MENA, Spirits Shop In Shop APAC, Spirits Shop In Shop Americas, Spirits Shop In Shop Europe, Spirits Shop In Shop MENA, Spirits Stand Alone Store APAC, Spirits Stand Alone Store Americas, Spirits Stand Alone Store Europe, Spirits Stand Alone Store MENA, 01_Primary Shelf (Bi-Weekly), 02_End Caps (Monthly), 03_Large HPP (Monthly), 04_HPP (Monthly), 05_On Shelf Availability (Biweekly)</t>
   </si>
   <si>
     <t xml:space="preserve">Include </t>
@@ -57,7 +60,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -87,13 +90,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="14"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -165,7 +161,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -182,11 +178,7 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -280,7 +272,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -295,7 +287,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1019" style="0" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="true" ht="45.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" s="4" customFormat="true" ht="45.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -311,7 +303,7 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="AME1" s="0"/>
@@ -322,24 +314,27 @@
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F1"/>
+  <autoFilter ref="A1:F2"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>